<commit_message>
Feature reduction from full product has been added.
</commit_message>
<xml_diff>
--- a/esg-engine/files/Cases/BankAccountPL/FullProductReduction/bankAccount.xlsx
+++ b/esg-engine/files/Cases/BankAccountPL/FullProductReduction/bankAccount.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="fullProduct_overdraft" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="71">
   <si>
     <t>Reduction Time(ms)</t>
   </si>
@@ -222,13 +222,31 @@
   </si>
   <si>
     <t>cancelDeposit, interestEstimation, dailyLimit</t>
+  </si>
+  <si>
+    <t>cancelWithdraw_credit_dailyLimit</t>
+  </si>
+  <si>
+    <t>cancelWithdraw_credit_interestEstimation</t>
+  </si>
+  <si>
+    <t>cancelWithdraw_interestEstimation_dailyLimit</t>
+  </si>
+  <si>
+    <t>credit_interest_interestEstimation</t>
+  </si>
+  <si>
+    <t>credit_interestEstimation_dailyLimit</t>
+  </si>
+  <si>
+    <t>interest_interestEstimation_dailyLimit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +296,28 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -287,7 +327,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -330,11 +370,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,9 +469,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -440,6 +514,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,10 +550,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,7 +588,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -752,33 +856,33 @@
       <selection activeCell="C17" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -807,7 +911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -836,7 +940,7 @@
         <v>6.81</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -865,7 +969,7 @@
         <v>6.85</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -894,7 +998,7 @@
         <v>7.91</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -923,7 +1027,7 @@
         <v>7.79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -952,7 +1056,7 @@
         <v>8.23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -981,7 +1085,7 @@
         <v>6.97</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1010,7 +1114,7 @@
         <v>7.19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1039,7 +1143,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1068,7 +1172,7 @@
         <v>7.89</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1097,7 +1201,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -1134,7 +1238,7 @@
         <v>7.3409999999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
@@ -1142,7 +1246,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
@@ -1150,8 +1254,8 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1179,8 +1283,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="48"/>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1206,8 +1310,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="48"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1223,8 +1327,8 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="48"/>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1256,29 +1360,29 @@
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="61.453125" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="1"/>
     <col min="14" max="14" width="44" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1318,12 +1422,12 @@
       <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="46"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="51"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
         <v>16</v>
       </c>
@@ -1419,7 +1523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>17</v>
       </c>
@@ -1460,12 +1564,12 @@
       <c r="N5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="44"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P5" s="49"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>18</v>
       </c>
@@ -1506,12 +1610,12 @@
       <c r="N6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="44" t="s">
+      <c r="O6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="44"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P6" s="49"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
@@ -1552,12 +1656,12 @@
       <c r="N7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="44" t="s">
+      <c r="O7" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="44"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7" s="49"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
         <v>20</v>
       </c>
@@ -1598,12 +1702,12 @@
       <c r="N8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="44" t="s">
+      <c r="O8" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="44"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P8" s="49"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
         <v>21</v>
       </c>
@@ -1651,7 +1755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="21" t="s">
         <v>22</v>
       </c>
@@ -1699,7 +1803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="21" t="s">
         <v>23</v>
       </c>
@@ -1740,12 +1844,12 @@
       <c r="N11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="44" t="s">
+      <c r="O11" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="44"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="49"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>24</v>
       </c>
@@ -1786,12 +1890,12 @@
       <c r="N12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="44" t="s">
+      <c r="O12" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="44"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12" s="49"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>31</v>
       </c>
@@ -1814,42 +1918,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K13"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="43.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="5" width="37.5703125" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" customWidth="1"/>
+    <col min="5" max="5" width="37.54296875" customWidth="1"/>
+    <col min="6" max="6" width="38.7265625" customWidth="1"/>
+    <col min="7" max="7" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.54296875" customWidth="1"/>
+    <col min="10" max="10" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="58"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -1868,23 +1978,35 @@
       <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="K2" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O2" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1903,23 +2025,35 @@
       <c r="F3" s="6">
         <v>7.93</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="42">
+        <v>7.99</v>
+      </c>
+      <c r="H3" s="42">
+        <v>9.23</v>
+      </c>
+      <c r="I3" s="6">
         <v>6.73</v>
       </c>
-      <c r="H3" s="6">
+      <c r="J3" s="6">
         <v>9.7899999999999991</v>
       </c>
-      <c r="I3" s="8">
+      <c r="K3" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="L3" s="8">
         <v>9.52</v>
       </c>
-      <c r="J3" s="11">
+      <c r="M3" s="11">
         <v>13.5</v>
       </c>
-      <c r="K3" s="8">
+      <c r="N3" s="8">
         <v>7.31</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O3" s="42">
+        <v>8.1300000000000008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -1938,23 +2072,35 @@
       <c r="F4" s="6">
         <v>14.24</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="42">
+        <v>7.56</v>
+      </c>
+      <c r="H4" s="42">
+        <v>8.16</v>
+      </c>
+      <c r="I4" s="6">
         <v>7.11</v>
       </c>
-      <c r="H4" s="6">
+      <c r="J4" s="6">
         <v>11.09</v>
       </c>
-      <c r="I4" s="8">
+      <c r="K4" s="42">
+        <v>8.4</v>
+      </c>
+      <c r="L4" s="8">
         <v>8.9700000000000006</v>
       </c>
-      <c r="J4" s="11">
+      <c r="M4" s="11">
         <v>7.59</v>
       </c>
-      <c r="K4" s="8">
+      <c r="N4" s="8">
         <v>7.15</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O4" s="42">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>3</v>
       </c>
@@ -1973,23 +2119,35 @@
       <c r="F5" s="6">
         <v>7.51</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="42">
+        <v>7.35</v>
+      </c>
+      <c r="H5" s="42">
+        <v>7.96</v>
+      </c>
+      <c r="I5" s="6">
         <v>6.92</v>
       </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
         <v>9.27</v>
       </c>
-      <c r="I5" s="8">
+      <c r="K5" s="42">
+        <v>7.92</v>
+      </c>
+      <c r="L5" s="8">
         <v>11.23</v>
       </c>
-      <c r="J5" s="11">
+      <c r="M5" s="11">
         <v>7.27</v>
       </c>
-      <c r="K5" s="8">
+      <c r="N5" s="8">
         <v>7.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O5" s="42">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2008,23 +2166,35 @@
       <c r="F6" s="6">
         <v>7.59</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="42">
+        <v>7.69</v>
+      </c>
+      <c r="H6" s="42">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I6" s="6">
         <v>9.5299999999999994</v>
       </c>
-      <c r="H6" s="6">
+      <c r="J6" s="6">
         <v>10.039999999999999</v>
       </c>
-      <c r="I6" s="8">
+      <c r="K6" s="42">
+        <v>7.89</v>
+      </c>
+      <c r="L6" s="8">
         <v>20.07</v>
       </c>
-      <c r="J6" s="11">
+      <c r="M6" s="11">
         <v>7.72</v>
       </c>
-      <c r="K6" s="8">
+      <c r="N6" s="8">
         <v>7.61</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O6" s="42">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -2043,23 +2213,35 @@
       <c r="F7" s="6">
         <v>6.45</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="42">
+        <v>9.27</v>
+      </c>
+      <c r="H7" s="42">
+        <v>7.36</v>
+      </c>
+      <c r="I7" s="6">
         <v>10.220000000000001</v>
       </c>
-      <c r="H7" s="6">
+      <c r="J7" s="6">
         <v>13.43</v>
       </c>
-      <c r="I7" s="8">
+      <c r="K7" s="42">
+        <v>7.5</v>
+      </c>
+      <c r="L7" s="8">
         <v>9.86</v>
       </c>
-      <c r="J7" s="11">
+      <c r="M7" s="11">
         <v>7.36</v>
       </c>
-      <c r="K7" s="8">
+      <c r="N7" s="8">
         <v>7.44</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O7" s="42">
+        <v>7.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -2078,23 +2260,35 @@
       <c r="F8" s="6">
         <v>7.04</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="42">
+        <v>9.48</v>
+      </c>
+      <c r="H8" s="42">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="I8" s="6">
         <v>7.06</v>
       </c>
-      <c r="H8" s="6">
+      <c r="J8" s="6">
         <v>22.12</v>
       </c>
-      <c r="I8" s="8">
+      <c r="K8" s="42">
+        <v>7.57</v>
+      </c>
+      <c r="L8" s="8">
         <v>9.43</v>
       </c>
-      <c r="J8" s="11">
+      <c r="M8" s="11">
         <v>7.07</v>
       </c>
-      <c r="K8" s="8">
+      <c r="N8" s="8">
         <v>7.49</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O8" s="42">
+        <v>7.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>7</v>
       </c>
@@ -2113,23 +2307,35 @@
       <c r="F9" s="6">
         <v>7.3</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="42">
+        <v>7.88</v>
+      </c>
+      <c r="H9" s="42">
+        <v>8.19</v>
+      </c>
+      <c r="I9" s="6">
         <v>6.65</v>
       </c>
-      <c r="H9" s="6">
+      <c r="J9" s="6">
         <v>9.3699999999999992</v>
       </c>
-      <c r="I9" s="8">
+      <c r="K9" s="42">
+        <v>7.63</v>
+      </c>
+      <c r="L9" s="8">
         <v>9.56</v>
       </c>
-      <c r="J9" s="11">
+      <c r="M9" s="11">
         <v>7.3</v>
       </c>
-      <c r="K9" s="8">
+      <c r="N9" s="8">
         <v>8.9700000000000006</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O9" s="42">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -2148,23 +2354,35 @@
       <c r="F10" s="6">
         <v>7.48</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="42">
+        <v>6.97</v>
+      </c>
+      <c r="H10" s="42">
+        <v>7.99</v>
+      </c>
+      <c r="I10" s="6">
         <v>9.6</v>
       </c>
-      <c r="H10" s="6">
+      <c r="J10" s="6">
         <v>9.9</v>
       </c>
-      <c r="I10" s="8">
+      <c r="K10" s="42">
+        <v>11.25</v>
+      </c>
+      <c r="L10" s="8">
         <v>9.07</v>
       </c>
-      <c r="J10" s="11">
+      <c r="M10" s="11">
         <v>7.66</v>
       </c>
-      <c r="K10" s="8">
+      <c r="N10" s="8">
         <v>7.09</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O10" s="42">
+        <v>9.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -2183,23 +2401,35 @@
       <c r="F11" s="6">
         <v>7.39</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="42">
+        <v>7.4</v>
+      </c>
+      <c r="H11" s="42">
+        <v>7.14</v>
+      </c>
+      <c r="I11" s="6">
         <v>7.45</v>
       </c>
-      <c r="H11" s="6">
+      <c r="J11" s="6">
         <v>9.89</v>
       </c>
-      <c r="I11" s="8">
+      <c r="K11" s="42">
+        <v>7.34</v>
+      </c>
+      <c r="L11" s="8">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J11" s="11">
+      <c r="M11" s="11">
         <v>7.14</v>
       </c>
-      <c r="K11" s="8">
+      <c r="N11" s="8">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O11" s="42">
+        <v>8.2200000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -2218,28 +2448,40 @@
       <c r="F12" s="6">
         <v>7.85</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="42">
+        <v>7.2</v>
+      </c>
+      <c r="H12" s="42">
+        <v>7.59</v>
+      </c>
+      <c r="I12" s="6">
         <v>7.16</v>
       </c>
-      <c r="H12" s="6">
+      <c r="J12" s="6">
         <v>13.58</v>
       </c>
-      <c r="I12" s="8">
+      <c r="K12" s="42">
+        <v>7.35</v>
+      </c>
+      <c r="L12" s="8">
         <v>9.69</v>
       </c>
-      <c r="J12" s="11">
+      <c r="M12" s="11">
         <v>8.36</v>
       </c>
-      <c r="K12" s="8">
+      <c r="N12" s="8">
         <v>6.92</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="42">
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="14">
-        <f t="shared" ref="B13:K13" si="0">AVERAGE(B3:B12)</f>
+        <f t="shared" ref="B13:N13" si="0">AVERAGE(B3:B12)</f>
         <v>10.003</v>
       </c>
       <c r="C13" s="5">
@@ -2258,33 +2500,54 @@
         <f t="shared" si="0"/>
         <v>8.0779999999999994</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="40">
+        <f>AVERAGE(G3:G12)</f>
+        <v>7.8790000000000022</v>
+      </c>
+      <c r="H13" s="40">
+        <f>AVERAGE(H3:H12)</f>
+        <v>8.1880000000000006</v>
+      </c>
+      <c r="I13" s="7">
         <f t="shared" si="0"/>
         <v>7.8429999999999991</v>
       </c>
-      <c r="H13" s="7">
+      <c r="J13" s="7">
         <f t="shared" si="0"/>
         <v>11.848000000000001</v>
       </c>
-      <c r="I13" s="7">
+      <c r="K13" s="40">
+        <f>AVERAGE(K3:K12)</f>
+        <v>8.0350000000000001</v>
+      </c>
+      <c r="L13" s="7">
         <f t="shared" si="0"/>
         <v>10.67</v>
       </c>
-      <c r="J13" s="7">
+      <c r="M13" s="7">
         <f t="shared" si="0"/>
         <v>8.0969999999999995</v>
       </c>
-      <c r="K13" s="7">
+      <c r="N13" s="7">
         <f t="shared" si="0"/>
         <v>7.5540000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O13" s="41">
+        <f>AVERAGE(O3:O12)</f>
+        <v>8.0540000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
+    </row>
+    <row r="19" spans="11:13" x14ac:dyDescent="0.35">
+      <c r="K19" s="44"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2299,32 +2562,32 @@
       <selection activeCell="K11" sqref="K11:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.81640625" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="47" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -2353,7 +2616,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2382,7 +2645,7 @@
         <v>7.38</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2411,7 +2674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -2440,7 +2703,7 @@
         <v>7.79</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -2469,7 +2732,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -2498,7 +2761,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -2527,7 +2790,7 @@
         <v>8.73</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -2556,7 +2819,7 @@
         <v>7.01</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -2585,7 +2848,7 @@
         <v>6.89</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -2614,7 +2877,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -2643,7 +2906,7 @@
         <v>7.51</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
@@ -2680,18 +2943,18 @@
         <v>7.6209999999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2722,8 +2985,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="48"/>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
@@ -2749,8 +3012,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="48"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
@@ -2776,8 +3039,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="48"/>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -2815,25 +3078,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
@@ -2858,13 +3128,34 @@
       <c r="H2" s="12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="13">
         <v>1</v>
       </c>
       <c r="B3" s="11">
-        <v>10.37</v>
+        <v>7.31</v>
       </c>
       <c r="C3" s="13">
         <v>7.4</v>
@@ -2884,13 +3175,34 @@
       <c r="H3" s="13">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="42">
+        <v>6.49</v>
+      </c>
+      <c r="J3" s="42">
+        <v>7.64</v>
+      </c>
+      <c r="K3" s="42">
+        <v>8.17</v>
+      </c>
+      <c r="L3" s="42">
+        <v>8.49</v>
+      </c>
+      <c r="M3" s="42">
+        <v>5.83</v>
+      </c>
+      <c r="N3" s="42">
+        <v>5.76</v>
+      </c>
+      <c r="O3" s="42">
+        <v>5.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" s="11">
-        <v>9.57</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="C4" s="13">
         <v>7.45</v>
@@ -2910,13 +3222,34 @@
       <c r="H4" s="13">
         <v>11.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="42">
+        <v>7.29</v>
+      </c>
+      <c r="J4" s="42">
+        <v>7.62</v>
+      </c>
+      <c r="K4" s="42">
+        <v>6.98</v>
+      </c>
+      <c r="L4" s="42">
+        <v>7.12</v>
+      </c>
+      <c r="M4" s="42">
+        <v>6.05</v>
+      </c>
+      <c r="N4" s="42">
+        <v>5.63</v>
+      </c>
+      <c r="O4" s="42">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" s="11">
-        <v>11.46</v>
+        <v>7.3</v>
       </c>
       <c r="C5" s="13">
         <v>7.34</v>
@@ -2936,13 +3269,34 @@
       <c r="H5" s="13">
         <v>6.96</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="42">
+        <v>5.56</v>
+      </c>
+      <c r="J5" s="42">
+        <v>7.1</v>
+      </c>
+      <c r="K5" s="42">
+        <v>7.81</v>
+      </c>
+      <c r="L5" s="42">
+        <v>6.04</v>
+      </c>
+      <c r="M5" s="42">
+        <v>5.84</v>
+      </c>
+      <c r="N5" s="42">
+        <v>6</v>
+      </c>
+      <c r="O5" s="42">
+        <v>7.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" s="11">
-        <v>14.89</v>
+        <v>8.31</v>
       </c>
       <c r="C6" s="13">
         <v>7.21</v>
@@ -2962,13 +3316,34 @@
       <c r="H6" s="13">
         <v>7.19</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="42">
+        <v>11.99</v>
+      </c>
+      <c r="J6" s="42">
+        <v>7.93</v>
+      </c>
+      <c r="K6" s="42">
+        <v>7.36</v>
+      </c>
+      <c r="L6" s="42">
+        <v>5.99</v>
+      </c>
+      <c r="M6" s="42">
+        <v>5.64</v>
+      </c>
+      <c r="N6" s="42">
+        <v>5.81</v>
+      </c>
+      <c r="O6" s="42">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" s="11">
-        <v>16.440000000000001</v>
+        <v>8.18</v>
       </c>
       <c r="C7" s="13">
         <v>7.52</v>
@@ -2988,13 +3363,34 @@
       <c r="H7" s="13">
         <v>7.11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="42">
+        <v>6.28</v>
+      </c>
+      <c r="J7" s="42">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="K7" s="42">
+        <v>7.32</v>
+      </c>
+      <c r="L7" s="42">
+        <v>5.16</v>
+      </c>
+      <c r="M7" s="42">
+        <v>5.91</v>
+      </c>
+      <c r="N7" s="42">
+        <v>5.54</v>
+      </c>
+      <c r="O7" s="42">
+        <v>5.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="13">
         <v>6</v>
       </c>
       <c r="B8" s="11">
-        <v>18.25</v>
+        <v>7.41</v>
       </c>
       <c r="C8" s="13">
         <v>7.01</v>
@@ -3014,13 +3410,34 @@
       <c r="H8" s="13">
         <v>7.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="42">
+        <v>5.93</v>
+      </c>
+      <c r="J8" s="42">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="K8" s="42">
+        <v>6.97</v>
+      </c>
+      <c r="L8" s="42">
+        <v>5.26</v>
+      </c>
+      <c r="M8" s="42">
+        <v>6.74</v>
+      </c>
+      <c r="N8" s="42">
+        <v>6.04</v>
+      </c>
+      <c r="O8" s="42">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>7</v>
       </c>
       <c r="B9" s="11">
-        <v>17.52</v>
+        <v>7.66</v>
       </c>
       <c r="C9" s="13">
         <v>7.63</v>
@@ -3040,13 +3457,34 @@
       <c r="H9" s="13">
         <v>7.13</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="42">
+        <v>6.09</v>
+      </c>
+      <c r="J9" s="42">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="K9" s="42">
+        <v>7.95</v>
+      </c>
+      <c r="L9" s="42">
+        <v>6.58</v>
+      </c>
+      <c r="M9" s="42">
+        <v>6.77</v>
+      </c>
+      <c r="N9" s="42">
+        <v>5.36</v>
+      </c>
+      <c r="O9" s="42">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>8</v>
       </c>
       <c r="B10" s="11">
-        <v>16.13</v>
+        <v>7.65</v>
       </c>
       <c r="C10" s="13">
         <v>7.68</v>
@@ -3066,13 +3504,34 @@
       <c r="H10" s="13">
         <v>7.46</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="42">
+        <v>6.43</v>
+      </c>
+      <c r="J10" s="42">
+        <v>7.42</v>
+      </c>
+      <c r="K10" s="42">
+        <v>7.52</v>
+      </c>
+      <c r="L10" s="42">
+        <v>5.94</v>
+      </c>
+      <c r="M10" s="42">
+        <v>5.7</v>
+      </c>
+      <c r="N10" s="42">
+        <v>6.51</v>
+      </c>
+      <c r="O10" s="42">
+        <v>5.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <v>9</v>
       </c>
       <c r="B11" s="11">
-        <v>13.85</v>
+        <v>8.06</v>
       </c>
       <c r="C11" s="13">
         <v>7.21</v>
@@ -3092,13 +3551,34 @@
       <c r="H11" s="13">
         <v>7.51</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="42">
+        <v>5.58</v>
+      </c>
+      <c r="J11" s="42">
+        <v>8.02</v>
+      </c>
+      <c r="K11" s="42">
+        <v>7.51</v>
+      </c>
+      <c r="L11" s="42">
+        <v>6.85</v>
+      </c>
+      <c r="M11" s="42">
+        <v>5.86</v>
+      </c>
+      <c r="N11" s="42">
+        <v>5.86</v>
+      </c>
+      <c r="O11" s="42">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="13">
         <v>10</v>
       </c>
       <c r="B12" s="11">
-        <v>11.51</v>
+        <v>8.16</v>
       </c>
       <c r="C12" s="13">
         <v>7.21</v>
@@ -3118,14 +3598,35 @@
       <c r="H12" s="13">
         <v>7.12</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="42">
+        <v>5.97</v>
+      </c>
+      <c r="J12" s="42">
+        <v>7.79</v>
+      </c>
+      <c r="K12" s="42">
+        <v>7.39</v>
+      </c>
+      <c r="L12" s="42">
+        <v>6.24</v>
+      </c>
+      <c r="M12" s="42">
+        <v>5.73</v>
+      </c>
+      <c r="N12" s="42">
+        <v>5.54</v>
+      </c>
+      <c r="O12" s="42">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="11">
         <f t="shared" ref="B13:H13" si="0">AVERAGE(B3:B12)</f>
-        <v>13.998999999999999</v>
+        <v>7.8249999999999984</v>
       </c>
       <c r="C13" s="11">
         <f t="shared" si="0"/>
@@ -3150,6 +3651,34 @@
       <c r="H13" s="13">
         <f t="shared" si="0"/>
         <v>7.8180000000000005</v>
+      </c>
+      <c r="I13" s="4">
+        <f>AVERAGE(I3:I12)</f>
+        <v>6.7610000000000001</v>
+      </c>
+      <c r="J13" s="4">
+        <f>AVERAGE(J3:J12)</f>
+        <v>8.0879999999999992</v>
+      </c>
+      <c r="K13" s="4">
+        <f>AVERAGE(K3:K12)</f>
+        <v>7.4980000000000002</v>
+      </c>
+      <c r="L13" s="4">
+        <f>AVERAGE(L3:L12)</f>
+        <v>6.3669999999999991</v>
+      </c>
+      <c r="M13" s="4">
+        <f>AVERAGE(M3:M12)</f>
+        <v>6.0070000000000006</v>
+      </c>
+      <c r="N13" s="4">
+        <f>AVERAGE(N3:N12)</f>
+        <v>5.8049999999999997</v>
+      </c>
+      <c r="O13" s="4">
+        <f>AVERAGE(O3:O12)</f>
+        <v>5.7660000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -3165,131 +3694,131 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="26">
         <v>3</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="26">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="26">
         <v>8</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="26">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="26">
         <v>8</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="26">
         <v>5</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="26">
         <v>5</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="26">
         <v>7</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="26">
         <v>6</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="26">
         <v>8</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="26">
         <v>8</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="26">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="26">
         <v>7</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <v>7</v>
       </c>
     </row>
@@ -3307,43 +3836,43 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="33">
         <v>20</v>
       </c>
-      <c r="C2" s="34">
+      <c r="C2" s="33">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="33">
         <v>21</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="33">
         <v>38</v>
       </c>
     </row>
@@ -3361,120 +3890,120 @@
       <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>9.24</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="24">
         <v>7.82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>10.43</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="24">
         <v>10.73</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>9.9</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="24">
         <v>10.41</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>10.66</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="24">
         <v>10.210000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>10.15</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="24">
         <v>10.81</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>7.2</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="24">
         <v>8.0299999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>9.7100000000000009</v>
       </c>
-      <c r="C11" s="25">
+      <c r="C11" s="24">
         <v>7.68</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="24">
         <v>7.34</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="25">
+      <c r="C13" s="24">
         <v>7.62</v>
       </c>
     </row>
@@ -3488,236 +4017,258 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7265625" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="55">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="55">
         <v>9.49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="55">
         <v>7.31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="55">
         <v>8.2100000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="55">
         <v>8.08</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="25"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="B8" s="55">
+        <v>7.8789999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="B9" s="54">
+        <v>8.1880000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="55">
         <v>7.84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="55">
         <v>11.85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="55">
         <v>10.67</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="B13" s="55">
+        <v>8.0350000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="55">
         <v>8.1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="39" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="55">
         <v>7.55</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="50" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="B16" s="55">
+        <v>8.0540000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="44"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="38">
-        <v>13.999000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
+      <c r="B20" s="37">
+        <v>7.8250000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="38">
+      <c r="B21" s="37">
         <v>7.3659999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="38">
+      <c r="B22" s="37">
         <v>9.81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="38">
+      <c r="B23" s="37">
         <v>7.9390000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="38">
+      <c r="B24" s="37">
         <v>7.532</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="38">
+      <c r="B25" s="37">
         <v>9.7889999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="38">
+      <c r="B26" s="37">
         <v>7.8179999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="22"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="B27" s="55">
+        <v>6.7610000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="22"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="B28" s="55">
+        <v>8.0879999999999992</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="22"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="B29" s="55">
+        <v>7.4980000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="22"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="48" t="s">
+      <c r="B30" s="55">
+        <v>6.367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="22"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="48" t="s">
+      <c r="B31" s="55">
+        <v>6.0069999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="22"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="48" t="s">
+      <c r="B32" s="55">
+        <v>5.8049999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="22"/>
+      <c r="B33" s="55">
+        <v>5.766</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Elimination conditions' result values have been updated.
</commit_message>
<xml_diff>
--- a/esg-engine/files/Cases/BankAccountPL/FullProductReduction/bankAccount.xlsx
+++ b/esg-engine/files/Cases/BankAccountPL/FullProductReduction/bankAccount.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="70">
   <si>
     <t>Reduction Time(ms)</t>
   </si>
@@ -197,12 +197,6 @@
     <t>cancelDeposit, credit, dailyLimit</t>
   </si>
   <si>
-    <t>fullProduct, overdraft</t>
-  </si>
-  <si>
-    <t>fullProduct, credit</t>
-  </si>
-  <si>
     <t>cancelWithdraw, credit, dailyLimit</t>
   </si>
   <si>
@@ -240,13 +234,16 @@
   </si>
   <si>
     <t>interest_interestEstimation_dailyLimit</t>
+  </si>
+  <si>
+    <t>fullProduct,_credit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,13 +292,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="162"/>
     </font>
     <font>
       <sz val="10"/>
@@ -507,9 +497,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -528,6 +515,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -546,30 +545,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -871,16 +861,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1255,7 +1245,7 @@
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="53" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1284,7 +1274,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="48"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1311,7 +1301,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="48"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1328,7 +1318,7 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="48"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1369,18 +1359,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -1422,10 +1412,10 @@
       <c r="N2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="50" t="s">
+      <c r="O2" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="51"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
@@ -1564,10 +1554,10 @@
       <c r="N5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="O5" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="49"/>
+      <c r="P5" s="54"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
@@ -1610,10 +1600,10 @@
       <c r="N6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="O6" s="49" t="s">
+      <c r="O6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="49"/>
+      <c r="P6" s="54"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
@@ -1656,10 +1646,10 @@
       <c r="N7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="49" t="s">
+      <c r="O7" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="49"/>
+      <c r="P7" s="54"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
@@ -1702,10 +1692,10 @@
       <c r="N8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="O8" s="49" t="s">
+      <c r="O8" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="49"/>
+      <c r="P8" s="54"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="21" t="s">
@@ -1844,10 +1834,10 @@
       <c r="N11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="49" t="s">
+      <c r="O11" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="49"/>
+      <c r="P11" s="54"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
@@ -1890,10 +1880,10 @@
       <c r="N12" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="49" t="s">
+      <c r="O12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="49"/>
+      <c r="P12" s="54"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
@@ -1943,21 +1933,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="59"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -1978,10 +1968,10 @@
       <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="47" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1990,8 +1980,8 @@
       <c r="J2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="60" t="s">
-        <v>67</v>
+      <c r="K2" s="47" t="s">
+        <v>65</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>22</v>
@@ -2003,7 +1993,7 @@
         <v>24</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -2025,10 +2015,10 @@
       <c r="F3" s="6">
         <v>7.93</v>
       </c>
-      <c r="G3" s="42">
+      <c r="G3" s="41">
         <v>7.99</v>
       </c>
-      <c r="H3" s="42">
+      <c r="H3" s="41">
         <v>9.23</v>
       </c>
       <c r="I3" s="6">
@@ -2037,7 +2027,7 @@
       <c r="J3" s="6">
         <v>9.7899999999999991</v>
       </c>
-      <c r="K3" s="42">
+      <c r="K3" s="41">
         <v>7.5</v>
       </c>
       <c r="L3" s="8">
@@ -2049,7 +2039,7 @@
       <c r="N3" s="8">
         <v>7.31</v>
       </c>
-      <c r="O3" s="42">
+      <c r="O3" s="41">
         <v>8.1300000000000008</v>
       </c>
     </row>
@@ -2072,10 +2062,10 @@
       <c r="F4" s="6">
         <v>14.24</v>
       </c>
-      <c r="G4" s="42">
+      <c r="G4" s="41">
         <v>7.56</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="41">
         <v>8.16</v>
       </c>
       <c r="I4" s="6">
@@ -2084,7 +2074,7 @@
       <c r="J4" s="6">
         <v>11.09</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="41">
         <v>8.4</v>
       </c>
       <c r="L4" s="8">
@@ -2096,7 +2086,7 @@
       <c r="N4" s="8">
         <v>7.15</v>
       </c>
-      <c r="O4" s="42">
+      <c r="O4" s="41">
         <v>8.07</v>
       </c>
     </row>
@@ -2119,10 +2109,10 @@
       <c r="F5" s="6">
         <v>7.51</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="41">
         <v>7.35</v>
       </c>
-      <c r="H5" s="42">
+      <c r="H5" s="41">
         <v>7.96</v>
       </c>
       <c r="I5" s="6">
@@ -2131,7 +2121,7 @@
       <c r="J5" s="6">
         <v>9.27</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="41">
         <v>7.92</v>
       </c>
       <c r="L5" s="8">
@@ -2143,7 +2133,7 @@
       <c r="N5" s="8">
         <v>7.36</v>
       </c>
-      <c r="O5" s="42">
+      <c r="O5" s="41">
         <v>8.5399999999999991</v>
       </c>
     </row>
@@ -2166,10 +2156,10 @@
       <c r="F6" s="6">
         <v>7.59</v>
       </c>
-      <c r="G6" s="42">
+      <c r="G6" s="41">
         <v>7.69</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="41">
         <v>9.8000000000000007</v>
       </c>
       <c r="I6" s="6">
@@ -2178,7 +2168,7 @@
       <c r="J6" s="6">
         <v>10.039999999999999</v>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="41">
         <v>7.89</v>
       </c>
       <c r="L6" s="8">
@@ -2190,7 +2180,7 @@
       <c r="N6" s="8">
         <v>7.61</v>
       </c>
-      <c r="O6" s="42">
+      <c r="O6" s="41">
         <v>7.23</v>
       </c>
     </row>
@@ -2213,10 +2203,10 @@
       <c r="F7" s="6">
         <v>6.45</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="41">
         <v>9.27</v>
       </c>
-      <c r="H7" s="42">
+      <c r="H7" s="41">
         <v>7.36</v>
       </c>
       <c r="I7" s="6">
@@ -2225,7 +2215,7 @@
       <c r="J7" s="6">
         <v>13.43</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="41">
         <v>7.5</v>
       </c>
       <c r="L7" s="8">
@@ -2237,7 +2227,7 @@
       <c r="N7" s="8">
         <v>7.44</v>
       </c>
-      <c r="O7" s="42">
+      <c r="O7" s="41">
         <v>7.86</v>
       </c>
     </row>
@@ -2260,10 +2250,10 @@
       <c r="F8" s="6">
         <v>7.04</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="41">
         <v>9.48</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="41">
         <v>8.4600000000000009</v>
       </c>
       <c r="I8" s="6">
@@ -2272,7 +2262,7 @@
       <c r="J8" s="6">
         <v>22.12</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="41">
         <v>7.57</v>
       </c>
       <c r="L8" s="8">
@@ -2284,7 +2274,7 @@
       <c r="N8" s="8">
         <v>7.49</v>
       </c>
-      <c r="O8" s="42">
+      <c r="O8" s="41">
         <v>7.56</v>
       </c>
     </row>
@@ -2307,10 +2297,10 @@
       <c r="F9" s="6">
         <v>7.3</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="41">
         <v>7.88</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="41">
         <v>8.19</v>
       </c>
       <c r="I9" s="6">
@@ -2319,7 +2309,7 @@
       <c r="J9" s="6">
         <v>9.3699999999999992</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="41">
         <v>7.63</v>
       </c>
       <c r="L9" s="8">
@@ -2331,7 +2321,7 @@
       <c r="N9" s="8">
         <v>8.9700000000000006</v>
       </c>
-      <c r="O9" s="42">
+      <c r="O9" s="41">
         <v>7.47</v>
       </c>
     </row>
@@ -2354,10 +2344,10 @@
       <c r="F10" s="6">
         <v>7.48</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="41">
         <v>6.97</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="41">
         <v>7.99</v>
       </c>
       <c r="I10" s="6">
@@ -2366,7 +2356,7 @@
       <c r="J10" s="6">
         <v>9.9</v>
       </c>
-      <c r="K10" s="42">
+      <c r="K10" s="41">
         <v>11.25</v>
       </c>
       <c r="L10" s="8">
@@ -2378,7 +2368,7 @@
       <c r="N10" s="8">
         <v>7.09</v>
       </c>
-      <c r="O10" s="42">
+      <c r="O10" s="41">
         <v>9.67</v>
       </c>
     </row>
@@ -2401,10 +2391,10 @@
       <c r="F11" s="6">
         <v>7.39</v>
       </c>
-      <c r="G11" s="42">
+      <c r="G11" s="41">
         <v>7.4</v>
       </c>
-      <c r="H11" s="42">
+      <c r="H11" s="41">
         <v>7.14</v>
       </c>
       <c r="I11" s="6">
@@ -2413,7 +2403,7 @@
       <c r="J11" s="6">
         <v>9.89</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="41">
         <v>7.34</v>
       </c>
       <c r="L11" s="8">
@@ -2425,7 +2415,7 @@
       <c r="N11" s="8">
         <v>8.1999999999999993</v>
       </c>
-      <c r="O11" s="42">
+      <c r="O11" s="41">
         <v>8.2200000000000006</v>
       </c>
     </row>
@@ -2448,10 +2438,10 @@
       <c r="F12" s="6">
         <v>7.85</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="41">
         <v>7.2</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="41">
         <v>7.59</v>
       </c>
       <c r="I12" s="6">
@@ -2460,7 +2450,7 @@
       <c r="J12" s="6">
         <v>13.58</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="41">
         <v>7.35</v>
       </c>
       <c r="L12" s="8">
@@ -2472,7 +2462,7 @@
       <c r="N12" s="8">
         <v>6.92</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="41">
         <v>7.79</v>
       </c>
     </row>
@@ -2500,11 +2490,11 @@
         <f t="shared" si="0"/>
         <v>8.0779999999999994</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="39">
         <f>AVERAGE(G3:G12)</f>
         <v>7.8790000000000022</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="39">
         <f>AVERAGE(H3:H12)</f>
         <v>8.1880000000000006</v>
       </c>
@@ -2516,7 +2506,7 @@
         <f t="shared" si="0"/>
         <v>11.848000000000001</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="39">
         <f>AVERAGE(K3:K12)</f>
         <v>8.0350000000000001</v>
       </c>
@@ -2532,7 +2522,7 @@
         <f t="shared" si="0"/>
         <v>7.5540000000000003</v>
       </c>
-      <c r="O13" s="41">
+      <c r="O13" s="40">
         <f>AVERAGE(O3:O12)</f>
         <v>8.0540000000000003</v>
       </c>
@@ -2541,9 +2531,9 @@
       <c r="B14" s="10"/>
     </row>
     <row r="19" spans="11:13" x14ac:dyDescent="0.35">
-      <c r="K19" s="44"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="44"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2576,16 +2566,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2954,7 +2944,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="53" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -2986,7 +2976,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="48"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
@@ -3013,7 +3003,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="48"/>
+      <c r="A18" s="53"/>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
@@ -3040,7 +3030,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="48"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
@@ -3128,26 +3118,26 @@
       <c r="H2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="M2" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="53" t="s">
+      <c r="N2" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="53" t="s">
+      <c r="O2" s="45" t="s">
         <v>68</v>
-      </c>
-      <c r="N2" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="O2" s="53" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -3175,25 +3165,25 @@
       <c r="H3" s="13">
         <v>8.9</v>
       </c>
-      <c r="I3" s="42">
+      <c r="I3" s="41">
         <v>6.49</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="41">
         <v>7.64</v>
       </c>
-      <c r="K3" s="42">
+      <c r="K3" s="41">
         <v>8.17</v>
       </c>
-      <c r="L3" s="42">
+      <c r="L3" s="41">
         <v>8.49</v>
       </c>
-      <c r="M3" s="42">
+      <c r="M3" s="41">
         <v>5.83</v>
       </c>
-      <c r="N3" s="42">
+      <c r="N3" s="41">
         <v>5.76</v>
       </c>
-      <c r="O3" s="42">
+      <c r="O3" s="41">
         <v>5.47</v>
       </c>
     </row>
@@ -3222,25 +3212,25 @@
       <c r="H4" s="13">
         <v>11.75</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="41">
         <v>7.29</v>
       </c>
-      <c r="J4" s="42">
+      <c r="J4" s="41">
         <v>7.62</v>
       </c>
-      <c r="K4" s="42">
+      <c r="K4" s="41">
         <v>6.98</v>
       </c>
-      <c r="L4" s="42">
+      <c r="L4" s="41">
         <v>7.12</v>
       </c>
-      <c r="M4" s="42">
+      <c r="M4" s="41">
         <v>6.05</v>
       </c>
-      <c r="N4" s="42">
+      <c r="N4" s="41">
         <v>5.63</v>
       </c>
-      <c r="O4" s="42">
+      <c r="O4" s="41">
         <v>5.15</v>
       </c>
     </row>
@@ -3269,25 +3259,25 @@
       <c r="H5" s="13">
         <v>6.96</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="41">
         <v>5.56</v>
       </c>
-      <c r="J5" s="42">
+      <c r="J5" s="41">
         <v>7.1</v>
       </c>
-      <c r="K5" s="42">
+      <c r="K5" s="41">
         <v>7.81</v>
       </c>
-      <c r="L5" s="42">
+      <c r="L5" s="41">
         <v>6.04</v>
       </c>
-      <c r="M5" s="42">
+      <c r="M5" s="41">
         <v>5.84</v>
       </c>
-      <c r="N5" s="42">
+      <c r="N5" s="41">
         <v>6</v>
       </c>
-      <c r="O5" s="42">
+      <c r="O5" s="41">
         <v>7.22</v>
       </c>
     </row>
@@ -3316,25 +3306,25 @@
       <c r="H6" s="13">
         <v>7.19</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="41">
         <v>11.99</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="41">
         <v>7.93</v>
       </c>
-      <c r="K6" s="42">
+      <c r="K6" s="41">
         <v>7.36</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="41">
         <v>5.99</v>
       </c>
-      <c r="M6" s="42">
+      <c r="M6" s="41">
         <v>5.64</v>
       </c>
-      <c r="N6" s="42">
+      <c r="N6" s="41">
         <v>5.81</v>
       </c>
-      <c r="O6" s="42">
+      <c r="O6" s="41">
         <v>5.58</v>
       </c>
     </row>
@@ -3363,25 +3353,25 @@
       <c r="H7" s="13">
         <v>7.11</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="41">
         <v>6.28</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="41">
         <v>8.6199999999999992</v>
       </c>
-      <c r="K7" s="42">
+      <c r="K7" s="41">
         <v>7.32</v>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="41">
         <v>5.16</v>
       </c>
-      <c r="M7" s="42">
+      <c r="M7" s="41">
         <v>5.91</v>
       </c>
-      <c r="N7" s="42">
+      <c r="N7" s="41">
         <v>5.54</v>
       </c>
-      <c r="O7" s="42">
+      <c r="O7" s="41">
         <v>5.63</v>
       </c>
     </row>
@@ -3410,25 +3400,25 @@
       <c r="H8" s="13">
         <v>7.05</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="41">
         <v>5.93</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="41">
         <v>9.2100000000000009</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="41">
         <v>6.97</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="41">
         <v>5.26</v>
       </c>
-      <c r="M8" s="42">
+      <c r="M8" s="41">
         <v>6.74</v>
       </c>
-      <c r="N8" s="42">
+      <c r="N8" s="41">
         <v>6.04</v>
       </c>
-      <c r="O8" s="42">
+      <c r="O8" s="41">
         <v>5.73</v>
       </c>
     </row>
@@ -3457,25 +3447,25 @@
       <c r="H9" s="13">
         <v>7.13</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="41">
         <v>6.09</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="41">
         <v>9.5299999999999994</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="41">
         <v>7.95</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="41">
         <v>6.58</v>
       </c>
-      <c r="M9" s="42">
+      <c r="M9" s="41">
         <v>6.77</v>
       </c>
-      <c r="N9" s="42">
+      <c r="N9" s="41">
         <v>5.36</v>
       </c>
-      <c r="O9" s="42">
+      <c r="O9" s="41">
         <v>5.56</v>
       </c>
     </row>
@@ -3504,25 +3494,25 @@
       <c r="H10" s="13">
         <v>7.46</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="41">
         <v>6.43</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="41">
         <v>7.42</v>
       </c>
-      <c r="K10" s="42">
+      <c r="K10" s="41">
         <v>7.52</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="41">
         <v>5.94</v>
       </c>
-      <c r="M10" s="42">
+      <c r="M10" s="41">
         <v>5.7</v>
       </c>
-      <c r="N10" s="42">
+      <c r="N10" s="41">
         <v>6.51</v>
       </c>
-      <c r="O10" s="42">
+      <c r="O10" s="41">
         <v>5.78</v>
       </c>
     </row>
@@ -3551,25 +3541,25 @@
       <c r="H11" s="13">
         <v>7.51</v>
       </c>
-      <c r="I11" s="42">
+      <c r="I11" s="41">
         <v>5.58</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="41">
         <v>8.02</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="41">
         <v>7.51</v>
       </c>
-      <c r="L11" s="42">
+      <c r="L11" s="41">
         <v>6.85</v>
       </c>
-      <c r="M11" s="42">
+      <c r="M11" s="41">
         <v>5.86</v>
       </c>
-      <c r="N11" s="42">
+      <c r="N11" s="41">
         <v>5.86</v>
       </c>
-      <c r="O11" s="42">
+      <c r="O11" s="41">
         <v>5.7</v>
       </c>
     </row>
@@ -3598,25 +3588,25 @@
       <c r="H12" s="13">
         <v>7.12</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="41">
         <v>5.97</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="41">
         <v>7.79</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="41">
         <v>7.39</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="41">
         <v>6.24</v>
       </c>
-      <c r="M12" s="42">
+      <c r="M12" s="41">
         <v>5.73</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12" s="41">
         <v>5.54</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="41">
         <v>5.84</v>
       </c>
     </row>
@@ -3653,31 +3643,31 @@
         <v>7.8180000000000005</v>
       </c>
       <c r="I13" s="4">
-        <f>AVERAGE(I3:I12)</f>
+        <f t="shared" ref="I13:O13" si="1">AVERAGE(I3:I12)</f>
         <v>6.7610000000000001</v>
       </c>
       <c r="J13" s="4">
-        <f>AVERAGE(J3:J12)</f>
+        <f t="shared" si="1"/>
         <v>8.0879999999999992</v>
       </c>
       <c r="K13" s="4">
-        <f>AVERAGE(K3:K12)</f>
+        <f t="shared" si="1"/>
         <v>7.4980000000000002</v>
       </c>
       <c r="L13" s="4">
-        <f>AVERAGE(L3:L12)</f>
+        <f t="shared" si="1"/>
         <v>6.3669999999999991</v>
       </c>
       <c r="M13" s="4">
-        <f>AVERAGE(M3:M12)</f>
+        <f t="shared" si="1"/>
         <v>6.0070000000000006</v>
       </c>
       <c r="N13" s="4">
-        <f>AVERAGE(N3:N12)</f>
+        <f t="shared" si="1"/>
         <v>5.8049999999999997</v>
       </c>
       <c r="O13" s="4">
-        <f>AVERAGE(O3:O12)</f>
+        <f t="shared" si="1"/>
         <v>5.7660000000000009</v>
       </c>
     </row>
@@ -4015,10 +4005,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B33"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4032,242 +4025,266 @@
         <v>40</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="49">
+        <v>9.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="49">
+        <v>7.31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="49">
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="49">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="49">
+        <v>7.8789999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="49">
+        <v>8.1880000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="49">
+        <v>7.84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="49">
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="49">
+        <v>10.67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="49">
+        <v>8.0350000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="49">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="49">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="49">
+        <v>8.0540000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="43"/>
+      <c r="B17" s="61">
+        <f>AVERAGE(B3:B16)</f>
+        <v>8.6611428571428561</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="43"/>
+      <c r="B18" s="61">
+        <f>MAX(B3:B16)</f>
+        <v>11.85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="43"/>
+      <c r="B19" s="10">
+        <f>MIN(B3:B16)</f>
+        <v>7.31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="50">
+        <v>7.8250000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="50">
+        <v>7.3659999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="50">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="50">
+        <v>7.9390000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="50">
+        <v>7.532</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="50">
+        <v>9.7889999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="50">
+        <v>7.8179999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="42" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="55">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="55">
-        <v>9.49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="55">
-        <v>7.31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="55">
-        <v>8.2100000000000009</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="55">
-        <v>8.08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="55">
-        <v>7.8789999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="54">
-        <v>8.1880000000000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="55">
-        <v>7.84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="38" t="s">
+      <c r="B29" s="49">
+        <v>6.7610000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="49">
+        <v>8.0879999999999992</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="55">
-        <v>11.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="55">
-        <v>10.67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+      <c r="B31" s="49">
+        <v>7.4980000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="49">
+        <v>6.367</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="49">
+        <v>6.0069999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="55">
-        <v>8.0350000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="55">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="55">
-        <v>7.55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="55">
-        <v>8.0540000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="37">
-        <v>7.8250000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="37">
-        <v>7.3659999999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="37">
-        <v>9.81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="37">
-        <v>7.9390000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="37">
-        <v>7.532</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="37">
-        <v>9.7889999999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="37">
-        <v>7.8179999999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="55">
-        <v>6.7610000000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="55">
-        <v>8.0879999999999992</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="55">
-        <v>7.4980000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="55">
-        <v>6.367</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
+      <c r="B34" s="49">
+        <v>5.8049999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="55">
-        <v>6.0069999999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="55">
-        <v>5.8049999999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="55">
+      <c r="B35" s="49">
         <v>5.766</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="10">
+        <f>AVERAGE(B22:B35)</f>
+        <v>7.4550714285714283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>